<commit_message>
Convert my insert only to an insert and update existing
</commit_message>
<xml_diff>
--- a/filmcab design.xlsx
+++ b/filmcab design.xlsx
@@ -8,8 +8,9 @@
   </bookViews>
   <sheets>
     <sheet name="Files" sheetId="1" r:id="rId2"/>
-    <sheet name="public figures" sheetId="2" r:id="rId3"/>
-    <sheet name="media_collections" sheetId="3" r:id="rId4"/>
+    <sheet name="people" sheetId="2" r:id="rId3"/>
+    <sheet name="public figures" sheetId="3" r:id="rId4"/>
+    <sheet name="media_collections" sheetId="4" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr fullCalcOnLoad="1"/>
@@ -17,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="94">
   <si>
     <t>Level 0</t>
   </si>
@@ -61,6 +62,9 @@
     <t>Relationship #3 Type</t>
   </si>
   <si>
+    <t>Relationship #3 Label</t>
+  </si>
+  <si>
     <t>Relationship #4</t>
   </si>
   <si>
@@ -76,49 +80,61 @@
     <t>Floating topic: Types</t>
   </si>
   <si>
+    <t>Floating topic: people</t>
+  </si>
+  <si>
+    <t>Floating topic: artists</t>
+  </si>
+  <si>
+    <t>Floating topic: Users</t>
+  </si>
+  <si>
+    <t>Floating topic: media_collections</t>
+  </si>
+  <si>
+    <t>Floating topic: studios</t>
+  </si>
+  <si>
+    <t>Floating topic: keys</t>
+  </si>
+  <si>
+    <t>Floating topic: tables</t>
+  </si>
+  <si>
+    <t>Floating topic: columns</t>
+  </si>
+  <si>
+    <t>Floating topic: annotations</t>
+  </si>
+  <si>
+    <t>Floating topic: reasons</t>
+  </si>
+  <si>
+    <t>Floating topic: tags</t>
+  </si>
+  <si>
+    <t>Floating topic: attributes</t>
+  </si>
+  <si>
+    <t>Floating topic: clips</t>
+  </si>
+  <si>
+    <t>Floating topic: quotes</t>
+  </si>
+  <si>
+    <t>Floating topic: cast_and_crew</t>
+  </si>
+  <si>
+    <t>Floating topic: subtitles</t>
+  </si>
+  <si>
+    <t>Floating topic: characters</t>
+  </si>
+  <si>
     <t>Floating topic: Urls</t>
   </si>
   <si>
-    <t>Floating topic: people</t>
-  </si>
-  <si>
-    <t>Floating topic: artists</t>
-  </si>
-  <si>
-    <t>Floating topic: Users</t>
-  </si>
-  <si>
-    <t>Floating topic: cast_and_crew</t>
-  </si>
-  <si>
-    <t>Floating topic: media_collections</t>
-  </si>
-  <si>
-    <t>Floating topic: studios</t>
-  </si>
-  <si>
-    <t>Floating topic: keys</t>
-  </si>
-  <si>
-    <t>Floating topic: tables</t>
-  </si>
-  <si>
-    <t>Floating topic: columns</t>
-  </si>
-  <si>
-    <t>Floating topic: annotations</t>
-  </si>
-  <si>
-    <t>Floating topic: reasons</t>
-  </si>
-  <si>
-    <t>Floating topic: tags</t>
-  </si>
-  <si>
-    <t>Floating topic: attributes</t>
-  </si>
-  <si>
-    <t>Floating topic: clips</t>
+    <t>Floating topic: genres</t>
   </si>
   <si>
     <t>media_files</t>
@@ -139,12 +155,12 @@
     <t>directories</t>
   </si>
   <si>
+    <t>public figures</t>
+  </si>
+  <si>
     <t>url_scan_history</t>
   </si>
   <si>
-    <t>public figures</t>
-  </si>
-  <si>
     <t>video_files</t>
   </si>
   <si>
@@ -184,58 +200,94 @@
     <t>media_collections</t>
   </si>
   <si>
+    <t>studios</t>
+  </si>
+  <si>
+    <t>artists</t>
+  </si>
+  <si>
+    <t>annotations</t>
+  </si>
+  <si>
+    <t>columns</t>
+  </si>
+  <si>
+    <t>tables</t>
+  </si>
+  <si>
+    <t>keys</t>
+  </si>
+  <si>
     <t>cast_and_crew</t>
   </si>
   <si>
-    <t>artists</t>
-  </si>
-  <si>
-    <t>annotations</t>
-  </si>
-  <si>
-    <t>columns</t>
-  </si>
-  <si>
-    <t>tables</t>
-  </si>
-  <si>
-    <t>keys</t>
-  </si>
-  <si>
     <t>Out</t>
   </si>
   <si>
     <t>In</t>
   </si>
   <si>
+    <t>Bi-directional</t>
+  </si>
+  <si>
+    <t>are a</t>
+  </si>
+  <si>
+    <t>contain</t>
+  </si>
+  <si>
+    <t>are made by</t>
+  </si>
+  <si>
+    <t>are</t>
+  </si>
+  <si>
     <t>have</t>
   </si>
   <si>
-    <t>are made by</t>
-  </si>
-  <si>
     <t>clipped from</t>
   </si>
   <si>
+    <t>play</t>
+  </si>
+  <si>
+    <t>pulled down from</t>
+  </si>
+  <si>
+    <t>Urls</t>
+  </si>
+  <si>
     <t>clips</t>
   </si>
   <si>
-    <t>studios</t>
-  </si>
-  <si>
     <t>people</t>
   </si>
   <si>
     <t>reasons</t>
   </si>
   <si>
-    <t>are</t>
+    <t>genres</t>
+  </si>
+  <si>
+    <t>subtitles</t>
   </si>
   <si>
     <t>tags</t>
   </si>
   <si>
+    <t>characters</t>
+  </si>
+  <si>
     <t>attributes</t>
+  </si>
+  <si>
+    <t>bare minimum in here. name, alternate name, user alias(es)</t>
+  </si>
+  <si>
+    <t>public figures table can be stuffed with public detail.</t>
+  </si>
+  <si>
+    <t>Notes of "people"</t>
   </si>
   <si>
     <t>Can have more detail about them legally.</t>
@@ -742,7 +794,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <dimension ref="A1:Q35"/>
+  <dimension ref="A1:R39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -766,13 +818,14 @@
     <col min="12" max="12" width="31.1428571428571" style="1"/>
     <col min="13" max="13" width="23.1428571428571" style="1"/>
     <col min="14" max="14" width="30.5714285714286" style="1"/>
-    <col min="15" max="15" width="23.1428571428571" style="1"/>
-    <col min="16" max="16" width="30.5714285714286" style="1"/>
-    <col min="17" max="17" width="26" style="1"/>
-    <col min="18" max="16384" width="9.14285714285714" style="1"/>
+    <col min="15" max="15" width="31.1428571428571" style="1"/>
+    <col min="16" max="16" width="23.1428571428571" style="1"/>
+    <col min="17" max="17" width="30.5714285714286" style="1"/>
+    <col min="18" max="18" width="26" style="1"/>
+    <col min="19" max="16384" width="9.14285714285714" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="18" customHeight="1">
+    <row r="1" spans="1:18" ht="18" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -824,112 +877,134 @@
       <c r="Q1" s="5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" ht="12.75" customHeight="1">
+      <c r="R1" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="12.75" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
+        <v>70</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>77</v>
+      </c>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
-    </row>
-    <row r="3" spans="1:17" ht="12.75" customHeight="1">
+      <c r="R2" s="1"/>
+    </row>
+    <row r="3" spans="1:18" ht="12.75" customHeight="1">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
+        <v>75</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
-    </row>
-    <row r="4" spans="1:17" ht="12.75" customHeight="1">
+      <c r="R3" s="1"/>
+    </row>
+    <row r="4" spans="1:18" ht="12.75" customHeight="1">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="J4" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="K4" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="K4" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="L4" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-      <c r="O4" s="1"/>
+        <v>72</v>
+      </c>
+      <c r="M4" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>74</v>
+      </c>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
-    </row>
-    <row r="5" spans="1:17" ht="12.75" customHeight="1">
+      <c r="R4" s="1"/>
+    </row>
+    <row r="5" spans="1:18" ht="12.75" customHeight="1">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -944,13 +1019,14 @@
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
-    </row>
-    <row r="6" spans="1:17" ht="12.75" customHeight="1">
+      <c r="R5" s="1"/>
+    </row>
+    <row r="6" spans="1:18" ht="12.75" customHeight="1">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -965,24 +1041,25 @@
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
-    </row>
-    <row r="7" spans="1:17" ht="12.75" customHeight="1">
+      <c r="R6" s="1"/>
+    </row>
+    <row r="7" spans="1:18" ht="12.75" customHeight="1">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="6" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
@@ -992,12 +1069,13 @@
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
-    </row>
-    <row r="8" spans="1:17" ht="12.75" customHeight="1">
+      <c r="R7" s="1"/>
+    </row>
+    <row r="8" spans="1:18" ht="12.75" customHeight="1">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -1013,13 +1091,14 @@
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
-    </row>
-    <row r="9" spans="1:17" ht="12.75" customHeight="1">
+      <c r="R8" s="1"/>
+    </row>
+    <row r="9" spans="1:18" ht="12.75" customHeight="1">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
@@ -1034,11 +1113,12 @@
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
-    </row>
-    <row r="10" spans="1:17" ht="12.75" customHeight="1">
+      <c r="R9" s="1"/>
+    </row>
+    <row r="10" spans="1:18" ht="12.75" customHeight="1">
       <c r="A10" s="1"/>
       <c r="B10" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -1055,11 +1135,12 @@
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
-    </row>
-    <row r="11" spans="1:17" ht="12.75" customHeight="1">
+      <c r="R10" s="1"/>
+    </row>
+    <row r="11" spans="1:18" ht="12.75" customHeight="1">
       <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -1076,11 +1157,12 @@
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
-    </row>
-    <row r="12" spans="1:17" ht="12.75" customHeight="1">
+      <c r="R11" s="1"/>
+    </row>
+    <row r="12" spans="1:18" ht="12.75" customHeight="1">
       <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -1097,17 +1179,18 @@
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
-    </row>
-    <row r="13" spans="1:17" ht="12.75" customHeight="1">
+      <c r="R12" s="1"/>
+    </row>
+    <row r="13" spans="1:18" ht="12.75" customHeight="1">
       <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
@@ -1120,11 +1203,12 @@
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
-    </row>
-    <row r="14" spans="1:17" ht="12.75" customHeight="1">
+      <c r="R13" s="1"/>
+    </row>
+    <row r="14" spans="1:18" ht="12.75" customHeight="1">
       <c r="A14" s="1"/>
       <c r="B14" s="1" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -1141,12 +1225,13 @@
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
       <c r="Q14" s="1"/>
-    </row>
-    <row r="15" spans="1:17" ht="12.75" customHeight="1">
+      <c r="R14" s="1"/>
+    </row>
+    <row r="15" spans="1:18" ht="12.75" customHeight="1">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -1162,13 +1247,14 @@
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
-    </row>
-    <row r="16" spans="1:17" ht="12.75" customHeight="1">
+      <c r="R15" s="1"/>
+    </row>
+    <row r="16" spans="1:18" ht="12.75" customHeight="1">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
@@ -1183,14 +1269,15 @@
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
       <c r="Q16" s="1"/>
-    </row>
-    <row r="17" spans="1:17" ht="12.75" customHeight="1">
+      <c r="R16" s="1"/>
+    </row>
+    <row r="17" spans="1:18" ht="12.75" customHeight="1">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
@@ -1204,10 +1291,11 @@
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
-    </row>
-    <row r="18" spans="1:17" ht="12.75" customHeight="1">
+      <c r="R17" s="1"/>
+    </row>
+    <row r="18" spans="1:18" ht="12.75" customHeight="1">
       <c r="A18" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1215,13 +1303,13 @@
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
@@ -1231,32 +1319,46 @@
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
-    </row>
-    <row r="19" spans="1:17" ht="12.75" customHeight="1">
+      <c r="R18" s="1"/>
+    </row>
+    <row r="19" spans="1:18" ht="12.75" customHeight="1">
       <c r="A19" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
+      <c r="G19" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="J19" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>67</v>
+      </c>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
-    </row>
-    <row r="20" spans="1:17" ht="12.75" customHeight="1">
+      <c r="R19" s="6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" ht="12.75" customHeight="1">
       <c r="A20" s="1"/>
       <c r="B20" s="1" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -1273,10 +1375,13 @@
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
       <c r="Q20" s="1"/>
-    </row>
-    <row r="21" spans="1:17" ht="12.75" customHeight="1">
+      <c r="R20" s="6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" ht="12.75" customHeight="1">
       <c r="A21" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1284,32 +1389,35 @@
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="6" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="I21" s="1"/>
+        <v>68</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>72</v>
+      </c>
       <c r="J21" s="6" t="s">
-        <v>56</v>
+        <v>80</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="M21" s="1"/>
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
       <c r="Q21" s="1"/>
-    </row>
-    <row r="22" spans="1:17" ht="12.75" customHeight="1">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1" t="s">
-        <v>41</v>
-      </c>
+      <c r="R21" s="1"/>
+    </row>
+    <row r="22" spans="1:18" ht="12.75" customHeight="1">
+      <c r="A22" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
@@ -1324,13 +1432,12 @@
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
-      <c r="Q22" s="6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" ht="12.75" customHeight="1">
+      <c r="Q22" s="1"/>
+      <c r="R22" s="1"/>
+    </row>
+    <row r="23" spans="1:18" ht="12.75" customHeight="1">
       <c r="A23" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1338,41 +1445,44 @@
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="6" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="J23" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="K23" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="L23" s="1" t="s">
-        <v>70</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
       <c r="M23" s="1"/>
       <c r="N23" s="1"/>
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
       <c r="Q23" s="1"/>
-    </row>
-    <row r="24" spans="1:17" ht="12.75" customHeight="1">
+      <c r="R23" s="6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" ht="12.75" customHeight="1">
       <c r="A24" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
+      <c r="G24" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>72</v>
+      </c>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
@@ -1381,10 +1491,11 @@
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
       <c r="Q24" s="1"/>
-    </row>
-    <row r="25" spans="1:17" ht="12.75" customHeight="1">
+      <c r="R24" s="1"/>
+    </row>
+    <row r="25" spans="1:18" ht="12.75" customHeight="1">
       <c r="A25" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1392,30 +1503,39 @@
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
       <c r="G25" s="6" t="s">
-        <v>42</v>
+        <v>62</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="J25" s="6" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="L25" s="1"/>
-      <c r="M25" s="1"/>
-      <c r="N25" s="1"/>
+      <c r="M25" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="N25" s="1" t="s">
+        <v>67</v>
+      </c>
       <c r="O25" s="1"/>
-      <c r="P25" s="1"/>
-      <c r="Q25" s="1"/>
-    </row>
-    <row r="26" spans="1:17" ht="12.75" customHeight="1">
+      <c r="P25" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q25" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="R25" s="1"/>
+    </row>
+    <row r="26" spans="1:18" ht="12.75" customHeight="1">
       <c r="A26" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1423,13 +1543,13 @@
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
       <c r="G26" s="6" t="s">
-        <v>34</v>
+        <v>63</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
@@ -1438,13 +1558,12 @@
       <c r="N26" s="1"/>
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
-      <c r="Q26" s="6" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" ht="12.75" customHeight="1">
+      <c r="Q26" s="1"/>
+      <c r="R26" s="1"/>
+    </row>
+    <row r="27" spans="1:18" ht="12.75" customHeight="1">
       <c r="A27" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -1452,13 +1571,13 @@
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
       <c r="G27" s="6" t="s">
-        <v>42</v>
+        <v>64</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
@@ -1468,10 +1587,11 @@
       <c r="O27" s="1"/>
       <c r="P27" s="1"/>
       <c r="Q27" s="1"/>
-    </row>
-    <row r="28" spans="1:17" ht="12.75" customHeight="1">
+      <c r="R27" s="1"/>
+    </row>
+    <row r="28" spans="1:18" ht="12.75" customHeight="1">
       <c r="A28" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -1479,38 +1599,27 @@
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
       <c r="G28" s="6" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="J28" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="K28" s="1" t="s">
-        <v>61</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
       <c r="L28" s="1"/>
-      <c r="M28" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="N28" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="O28" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="P28" s="1" t="s">
-        <v>61</v>
-      </c>
+      <c r="M28" s="1"/>
+      <c r="N28" s="1"/>
+      <c r="O28" s="1"/>
+      <c r="P28" s="1"/>
       <c r="Q28" s="1"/>
-    </row>
-    <row r="29" spans="1:17" ht="12.75" customHeight="1">
+      <c r="R28" s="1"/>
+    </row>
+    <row r="29" spans="1:18" ht="12.75" customHeight="1">
       <c r="A29" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -1518,14 +1627,12 @@
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
       <c r="G29" s="6" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="I29" s="1" t="s">
-        <v>63</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="I29" s="1"/>
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
@@ -1534,10 +1641,11 @@
       <c r="O29" s="1"/>
       <c r="P29" s="1"/>
       <c r="Q29" s="1"/>
-    </row>
-    <row r="30" spans="1:17" ht="12.75" customHeight="1">
+      <c r="R29" s="1"/>
+    </row>
+    <row r="30" spans="1:18" ht="12.75" customHeight="1">
       <c r="A30" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -1545,14 +1653,12 @@
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
       <c r="G30" s="6" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="I30" s="1" t="s">
-        <v>63</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="I30" s="1"/>
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
@@ -1561,10 +1667,11 @@
       <c r="O30" s="1"/>
       <c r="P30" s="1"/>
       <c r="Q30" s="1"/>
-    </row>
-    <row r="31" spans="1:17" ht="12.75" customHeight="1">
+      <c r="R30" s="1"/>
+    </row>
+    <row r="31" spans="1:18" ht="12.75" customHeight="1">
       <c r="A31" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -1572,14 +1679,12 @@
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
       <c r="G31" s="6" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="I31" s="1" t="s">
-        <v>63</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="I31" s="1"/>
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
@@ -1588,10 +1693,11 @@
       <c r="O31" s="1"/>
       <c r="P31" s="1"/>
       <c r="Q31" s="1"/>
-    </row>
-    <row r="32" spans="1:17" ht="12.75" customHeight="1">
+      <c r="R31" s="1"/>
+    </row>
+    <row r="32" spans="1:18" ht="12.75" customHeight="1">
       <c r="A32" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -1599,12 +1705,14 @@
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
       <c r="G32" s="6" t="s">
-        <v>60</v>
+        <v>39</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="I32" s="1"/>
+        <v>67</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>75</v>
+      </c>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
@@ -1613,22 +1721,19 @@
       <c r="O32" s="1"/>
       <c r="P32" s="1"/>
       <c r="Q32" s="1"/>
-    </row>
-    <row r="33" spans="1:17" ht="12.75" customHeight="1">
+      <c r="R32" s="1"/>
+    </row>
+    <row r="33" spans="1:18" ht="12.75" customHeight="1">
       <c r="A33" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
-      <c r="G33" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="H33" s="1" t="s">
-        <v>62</v>
-      </c>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
@@ -1638,10 +1743,11 @@
       <c r="O33" s="1"/>
       <c r="P33" s="1"/>
       <c r="Q33" s="1"/>
-    </row>
-    <row r="34" spans="1:17" ht="12.75" customHeight="1">
+      <c r="R33" s="1"/>
+    </row>
+    <row r="34" spans="1:18" ht="12.75" customHeight="1">
       <c r="A34" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -1649,24 +1755,37 @@
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
       <c r="G34" s="6" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="I34" s="1"/>
-      <c r="J34" s="1"/>
-      <c r="K34" s="1"/>
+        <v>68</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J34" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="K34" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="L34" s="1"/>
-      <c r="M34" s="1"/>
-      <c r="N34" s="1"/>
-      <c r="O34" s="1"/>
+      <c r="M34" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="N34" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="O34" s="1" t="s">
+        <v>76</v>
+      </c>
       <c r="P34" s="1"/>
       <c r="Q34" s="1"/>
-    </row>
-    <row r="35" spans="1:17" ht="12.75" customHeight="1">
+      <c r="R34" s="1"/>
+    </row>
+    <row r="35" spans="1:18" ht="12.75" customHeight="1">
       <c r="A35" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -1674,13 +1793,13 @@
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
       <c r="G35" s="6" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
@@ -1690,37 +1809,151 @@
       <c r="O35" s="1"/>
       <c r="P35" s="1"/>
       <c r="Q35" s="1"/>
+      <c r="R35" s="1"/>
+    </row>
+    <row r="36" spans="1:18" ht="12.75" customHeight="1">
+      <c r="A36" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="J36" s="1"/>
+      <c r="K36" s="1"/>
+      <c r="L36" s="1"/>
+      <c r="M36" s="1"/>
+      <c r="N36" s="1"/>
+      <c r="O36" s="1"/>
+      <c r="P36" s="1"/>
+      <c r="Q36" s="1"/>
+      <c r="R36" s="1"/>
+    </row>
+    <row r="37" spans="1:18" ht="12.75" customHeight="1">
+      <c r="A37" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="J37" s="1"/>
+      <c r="K37" s="1"/>
+      <c r="L37" s="1"/>
+      <c r="M37" s="1"/>
+      <c r="N37" s="1"/>
+      <c r="O37" s="1"/>
+      <c r="P37" s="1"/>
+      <c r="Q37" s="1"/>
+      <c r="R37" s="1"/>
+    </row>
+    <row r="38" spans="1:18" ht="12.75" customHeight="1">
+      <c r="A38" s="1"/>
+      <c r="B38" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1"/>
+      <c r="K38" s="1"/>
+      <c r="L38" s="1"/>
+      <c r="M38" s="1"/>
+      <c r="N38" s="1"/>
+      <c r="O38" s="1"/>
+      <c r="P38" s="1"/>
+      <c r="Q38" s="1"/>
+      <c r="R38" s="1"/>
+    </row>
+    <row r="39" spans="1:18" ht="12.75" customHeight="1">
+      <c r="A39" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="I39" s="1"/>
+      <c r="J39" s="1"/>
+      <c r="K39" s="1"/>
+      <c r="L39" s="1"/>
+      <c r="M39" s="1"/>
+      <c r="N39" s="1"/>
+      <c r="O39" s="1"/>
+      <c r="P39" s="1"/>
+      <c r="Q39" s="1"/>
+      <c r="R39" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G2" location="'Files'!A18" display="Types"/>
-    <hyperlink ref="G3" location="'Files'!A26" display="media_collections"/>
-    <hyperlink ref="G4" location="'Files'!A25" display="cast_and_crew"/>
-    <hyperlink ref="G7" location="'Files'!A23" display="artists"/>
+    <hyperlink ref="G3" location="'Files'!A23" display="media_collections"/>
+    <hyperlink ref="G4" location="'Files'!A24" display="studios"/>
+    <hyperlink ref="G7" location="'Files'!A21" display="artists"/>
     <hyperlink ref="G18" location="'Files'!A2" display="Files"/>
-    <hyperlink ref="G21" location="'Files'!A25" display="cast_and_crew"/>
-    <hyperlink ref="G23" location="'Files'!C7" display="audio_files"/>
-    <hyperlink ref="G25" location="'Files'!C4" display="video_files"/>
-    <hyperlink ref="G26" location="'Files'!B3" display="media_files"/>
-    <hyperlink ref="G27" location="'Files'!C4" display="video_files"/>
-    <hyperlink ref="G28" location="'Files'!A31" display="annotations"/>
-    <hyperlink ref="G29" location="'Files'!A30" display="columns"/>
-    <hyperlink ref="G30" location="'Files'!A29" display="tables"/>
-    <hyperlink ref="G31" location="'Files'!A28" display="keys"/>
-    <hyperlink ref="G32" location="'Files'!A28" display="keys"/>
-    <hyperlink ref="G33" location="'Files'!A28" display="keys"/>
-    <hyperlink ref="G34" location="'Files'!A28" display="keys"/>
-    <hyperlink ref="G35" location="'Files'!B3" display="media_files"/>
-    <hyperlink ref="J3" location="'Files'!A35" display="clips"/>
-    <hyperlink ref="J4" location="'Files'!A27" display="studios"/>
-    <hyperlink ref="J21" location="'Files'!A23" display="artists"/>
-    <hyperlink ref="J23" location="'Files'!A21" display="people"/>
-    <hyperlink ref="J25" location="'Files'!A21" display="people"/>
-    <hyperlink ref="J28" location="'Files'!A32" display="reasons"/>
-    <hyperlink ref="M28" location="'Files'!A33" display="tags"/>
-    <hyperlink ref="O28" location="'Files'!A34" display="attributes"/>
-    <hyperlink ref="Q22" location="'public figures'!A1" display="Notes of &quot;public figures&quot;"/>
-    <hyperlink ref="Q26" location="'media_collections'!A1" display="Notes of &quot;media_collections&quot;"/>
+    <hyperlink ref="G19" location="'Files'!A21" display="artists"/>
+    <hyperlink ref="G21" location="'Files'!C7" display="audio_files"/>
+    <hyperlink ref="G23" location="'Files'!B3" display="media_files"/>
+    <hyperlink ref="G24" location="'Files'!C4" display="video_files"/>
+    <hyperlink ref="G25" location="'Files'!A28" display="annotations"/>
+    <hyperlink ref="G26" location="'Files'!A27" display="columns"/>
+    <hyperlink ref="G27" location="'Files'!A26" display="tables"/>
+    <hyperlink ref="G28" location="'Files'!A25" display="keys"/>
+    <hyperlink ref="G29" location="'Files'!A25" display="keys"/>
+    <hyperlink ref="G30" location="'Files'!A25" display="keys"/>
+    <hyperlink ref="G31" location="'Files'!A25" display="keys"/>
+    <hyperlink ref="G32" location="'Files'!B3" display="media_files"/>
+    <hyperlink ref="G34" location="'Files'!C4" display="video_files"/>
+    <hyperlink ref="G35" location="'Files'!C4" display="video_files"/>
+    <hyperlink ref="G36" location="'Files'!A34" display="cast_and_crew"/>
+    <hyperlink ref="G37" location="'Files'!A2" display="Files"/>
+    <hyperlink ref="G39" location="'Files'!B3" display="media_files"/>
+    <hyperlink ref="J2" location="'Files'!A37" display="Urls"/>
+    <hyperlink ref="J3" location="'Files'!A32" display="clips"/>
+    <hyperlink ref="J4" location="'Files'!A34" display="cast_and_crew"/>
+    <hyperlink ref="J19" location="'Files'!A34" display="cast_and_crew"/>
+    <hyperlink ref="J21" location="'Files'!A19" display="people"/>
+    <hyperlink ref="J25" location="'Files'!A29" display="reasons"/>
+    <hyperlink ref="J34" location="'Files'!A19" display="people"/>
+    <hyperlink ref="M3" location="'Files'!A39" display="genres"/>
+    <hyperlink ref="M4" location="'Files'!A35" display="subtitles"/>
+    <hyperlink ref="M25" location="'Files'!A30" display="tags"/>
+    <hyperlink ref="M34" location="'Files'!A36" display="characters"/>
+    <hyperlink ref="P25" location="'Files'!A31" display="attributes"/>
+    <hyperlink ref="R19" location="'people'!A1" display="Notes of &quot;people&quot;"/>
+    <hyperlink ref="R20" location="'public figures'!A1" display="Notes of &quot;public figures&quot;"/>
+    <hyperlink ref="R23" location="'media_collections'!A1" display="Notes of &quot;media_collections&quot;"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait"/>
@@ -1729,7 +1962,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0" topLeftCell="A1"/>
   </sheetViews>
@@ -1737,7 +1970,12 @@
   <sheetData>
     <row r="1" spans="1:1" ht="12.75">
       <c r="A1" s="7" t="s">
-        <v>73</v>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="12.75">
+      <c r="A2" s="7" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -1756,7 +1994,26 @@
   <sheetData>
     <row r="1" spans="1:1" ht="12.75">
       <c r="A1" s="7" t="s">
-        <v>75</v>
+        <v>90</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0" topLeftCell="A1"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetData>
+    <row r="1" spans="1:1" ht="12.75">
+      <c r="A1" s="7" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>